<commit_message>
Correção de bug (leitura de casas decimais das frequências) e documentação.
</commit_message>
<xml_diff>
--- a/DataBase/FM.xlsx
+++ b/DataBase/FM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ericmdelgado.ANATEL\Downloads\RFEye\DataBase\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\OneDrive - ANATEL\appAnalise\DataBase\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73DD27AF-5744-4F33-92EA-014FD70DCCD6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="49170" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12698,7 +12698,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.000000"/>
+    <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -12731,8 +12731,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -13064,7 +13064,7 @@
   <dimension ref="A1:E4220"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22669" sqref="A22669"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -84824,6 +84824,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100A3E2CBE5199FE342B4D267176DE65E53" ma:contentTypeVersion="7" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="0accf7910c01a6b9d6bc16452487f933">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="129b23b4-ac31-4ca9-81eb-f757e3f2b6b4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bd659eee9ea884cf2ee542adada12c87" ns2:_="">
     <xsd:import namespace="129b23b4-ac31-4ca9-81eb-f757e3f2b6b4"/>
@@ -84987,29 +85002,44 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{207E747F-761A-4FCE-9E9A-EA89EABA889A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29A0CEB4-83DA-4F35-B3D1-2AB8A6EAE048}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="129b23b4-ac31-4ca9-81eb-f757e3f2b6b4"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB34916B-3BA0-40E9-9E6C-F224B9A0A562}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB34916B-3BA0-40E9-9E6C-F224B9A0A562}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29A0CEB4-83DA-4F35-B3D1-2AB8A6EAE048}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{207E747F-761A-4FCE-9E9A-EA89EABA889A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="129b23b4-ac31-4ca9-81eb-f757e3f2b6b4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>